<commit_message>
Replacing the corrected NFS DATA excel
The previous NFS data had been replaced with previous versions, it has been corrected again
</commit_message>
<xml_diff>
--- a/NFSData/NFS Data.xlsx
+++ b/NFSData/NFS Data.xlsx
@@ -5,11 +5,12 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\A.H.Kh\HomeWork\03-Practical Projects\AFDNFS\AFDNFS v1.0.0.19\NFSData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\A.H.Kh\HomeWork\03-Practical Projects\AFDNFS\AFDNFS Git\NFSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="M0R0OALV+6f4UVn5GwSJvjPKd6y0Z7YAv336xc5+wD0694sFyycXUoMm4kQWjCbyA7IyUV/m+S/8rCX45lhMVg==" workbookSaltValue="i7Ezyq5BRvQUEGVk7PYG3A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23976" windowHeight="10260" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23976" windowHeight="10260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AFD NFS" sheetId="4" r:id="rId1"/>
@@ -17,9 +18,6 @@
     <sheet name="NFS Cruise - Aerodynamics Data" sheetId="2" r:id="rId3"/>
     <sheet name="Prefered Data Sets" sheetId="5" state="hidden" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Units">'Prefered Data Sets'!$B$1:$B$2</definedName>
   </definedNames>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="88">
   <si>
     <t>Aerodynamic Mean Chord</t>
   </si>
@@ -68,232 +66,235 @@
     <t>Initial Altitude</t>
   </si>
   <si>
+    <t>Initial Cruse Velocity</t>
+  </si>
+  <si>
+    <t>MOI Tensor</t>
+  </si>
+  <si>
+    <t>Initial Attitude</t>
+  </si>
+  <si>
+    <t>Initial Angular Velocities</t>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t>NFS General Data</t>
+  </si>
+  <si>
+    <t>NFS Aerodynamic Coefficients - Cruise</t>
+  </si>
+  <si>
+    <t>Stability Derivatives</t>
+  </si>
+  <si>
+    <t>Longitudinal</t>
+  </si>
+  <si>
+    <t>CD1</t>
+  </si>
+  <si>
+    <t>CD0</t>
+  </si>
+  <si>
+    <t>CDu</t>
+  </si>
+  <si>
+    <t>CDalpha</t>
+  </si>
+  <si>
+    <t>CDM</t>
+  </si>
+  <si>
+    <t>CTx1</t>
+  </si>
+  <si>
+    <t>CTxu</t>
+  </si>
+  <si>
+    <t>CL1</t>
+  </si>
+  <si>
+    <t>CL0</t>
+  </si>
+  <si>
+    <t>CLu</t>
+  </si>
+  <si>
+    <t>CLalpha</t>
+  </si>
+  <si>
+    <t>CLalphadot</t>
+  </si>
+  <si>
+    <t>CLq</t>
+  </si>
+  <si>
+    <t>CLM</t>
+  </si>
+  <si>
+    <t>Cm1</t>
+  </si>
+  <si>
+    <t>Cm0</t>
+  </si>
+  <si>
+    <t>Cmu</t>
+  </si>
+  <si>
+    <t>Cmalpha</t>
+  </si>
+  <si>
+    <t>Cmalphadot</t>
+  </si>
+  <si>
+    <t>Cmq</t>
+  </si>
+  <si>
+    <t>CmT1</t>
+  </si>
+  <si>
+    <t>CmTu</t>
+  </si>
+  <si>
+    <t>CmTalpha</t>
+  </si>
+  <si>
+    <t>CmM</t>
+  </si>
+  <si>
+    <t>CYbeta</t>
+  </si>
+  <si>
+    <t>CYbetadot</t>
+  </si>
+  <si>
+    <t>CYp</t>
+  </si>
+  <si>
+    <t>CYr</t>
+  </si>
+  <si>
+    <t>Clbeta</t>
+  </si>
+  <si>
+    <t>Clbetadot</t>
+  </si>
+  <si>
+    <t>Clp</t>
+  </si>
+  <si>
+    <t>Clr</t>
+  </si>
+  <si>
+    <t>Cnbeta</t>
+  </si>
+  <si>
+    <t>Cnbetadot</t>
+  </si>
+  <si>
+    <t>Cnp</t>
+  </si>
+  <si>
+    <t>Cnr</t>
+  </si>
+  <si>
+    <t>CnTbeta</t>
+  </si>
+  <si>
+    <t>Control Derivatives</t>
+  </si>
+  <si>
+    <t>CDdelta_e</t>
+  </si>
+  <si>
+    <t>CDdelta_f</t>
+  </si>
+  <si>
+    <t>CDdelta_a</t>
+  </si>
+  <si>
+    <t>CDdelta_r</t>
+  </si>
+  <si>
+    <t>CLdelta_e</t>
+  </si>
+  <si>
+    <t>CLdelta_f</t>
+  </si>
+  <si>
+    <t>Cmdelta_e</t>
+  </si>
+  <si>
+    <t>Cmdelta_f</t>
+  </si>
+  <si>
+    <t>Lateral - Directional</t>
+  </si>
+  <si>
+    <t>CYdelta_a</t>
+  </si>
+  <si>
+    <t>CYdelta_r</t>
+  </si>
+  <si>
+    <t>Cldelta_a</t>
+  </si>
+  <si>
+    <t>Cldelta_r</t>
+  </si>
+  <si>
+    <t>Cndelta_a</t>
+  </si>
+  <si>
+    <t>Cndelta_r</t>
+  </si>
+  <si>
+    <t>CDiH</t>
+  </si>
+  <si>
+    <t>CLiH</t>
+  </si>
+  <si>
+    <t>CMiH</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Allowable System of Units</t>
+  </si>
+  <si>
+    <t>Imperial</t>
+  </si>
+  <si>
+    <t>Advanced Flight Dynamics - Nonlinear Flight Simulation</t>
+  </si>
+  <si>
+    <t>Current Version</t>
+  </si>
+  <si>
+    <t>System of Units</t>
+  </si>
+  <si>
+    <t>Advanced Flight Dynamics Nonlinear Flight Simulation is a comprehencive flight simulation (the Software simulation must goes here) …</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1/rad</t>
+  </si>
+  <si>
+    <t>MOI Tensor Rate</t>
+  </si>
+  <si>
     <t>Initial Weight</t>
   </si>
   <si>
-    <t>Initial Cruse Velocity</t>
-  </si>
-  <si>
-    <t>MOI Tensor</t>
-  </si>
-  <si>
-    <t>Initial Attitude</t>
-  </si>
-  <si>
-    <t>Initial Angular Velocities</t>
-  </si>
-  <si>
-    <t>rad</t>
-  </si>
-  <si>
-    <t>NFS General Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>NFS Aerodynamic Coefficients - Cruise</t>
-  </si>
-  <si>
-    <t>Stability Derivatives</t>
-  </si>
-  <si>
-    <t>Longitudinal</t>
-  </si>
-  <si>
-    <t>CD1</t>
-  </si>
-  <si>
-    <t>CD0</t>
-  </si>
-  <si>
-    <t>CDu</t>
-  </si>
-  <si>
-    <t>CDalpha</t>
-  </si>
-  <si>
-    <t>CDM</t>
-  </si>
-  <si>
-    <t>CTx1</t>
-  </si>
-  <si>
-    <t>CTxu</t>
-  </si>
-  <si>
-    <t>CL1</t>
-  </si>
-  <si>
-    <t>CL0</t>
-  </si>
-  <si>
-    <t>CLu</t>
-  </si>
-  <si>
-    <t>CLalpha</t>
-  </si>
-  <si>
-    <t>CLalphadot</t>
-  </si>
-  <si>
-    <t>CLq</t>
-  </si>
-  <si>
-    <t>CLM</t>
-  </si>
-  <si>
-    <t>Cm1</t>
-  </si>
-  <si>
-    <t>Cm0</t>
-  </si>
-  <si>
-    <t>Cmu</t>
-  </si>
-  <si>
-    <t>Cmalpha</t>
-  </si>
-  <si>
-    <t>Cmalphadot</t>
-  </si>
-  <si>
-    <t>Cmq</t>
-  </si>
-  <si>
-    <t>CmT1</t>
-  </si>
-  <si>
-    <t>CmTu</t>
-  </si>
-  <si>
-    <t>CmTalpha</t>
-  </si>
-  <si>
-    <t>CmM</t>
-  </si>
-  <si>
-    <t>CYbeta</t>
-  </si>
-  <si>
-    <t>CYbetadot</t>
-  </si>
-  <si>
-    <t>CYp</t>
-  </si>
-  <si>
-    <t>CYr</t>
-  </si>
-  <si>
-    <t>Clbeta</t>
-  </si>
-  <si>
-    <t>Clbetadot</t>
-  </si>
-  <si>
-    <t>Clp</t>
-  </si>
-  <si>
-    <t>Clr</t>
-  </si>
-  <si>
-    <t>Cnbeta</t>
-  </si>
-  <si>
-    <t>Cnbetadot</t>
-  </si>
-  <si>
-    <t>Cnp</t>
-  </si>
-  <si>
-    <t>Cnr</t>
-  </si>
-  <si>
-    <t>CnTbeta</t>
-  </si>
-  <si>
-    <t>Control Derivatives</t>
-  </si>
-  <si>
-    <t>CDdelta_e</t>
-  </si>
-  <si>
-    <t>CDdelta_f</t>
-  </si>
-  <si>
-    <t>CDdelta_a</t>
-  </si>
-  <si>
-    <t>CDdelta_r</t>
-  </si>
-  <si>
-    <t>CLdelta_e</t>
-  </si>
-  <si>
-    <t>CLdelta_f</t>
-  </si>
-  <si>
-    <t>Cmdelta_e</t>
-  </si>
-  <si>
-    <t>Cmdelta_f</t>
-  </si>
-  <si>
-    <t>Lateral - Directional</t>
-  </si>
-  <si>
-    <t>CYdelta_a</t>
-  </si>
-  <si>
-    <t>CYdelta_r</t>
-  </si>
-  <si>
-    <t>Cldelta_a</t>
-  </si>
-  <si>
-    <t>Cldelta_r</t>
-  </si>
-  <si>
-    <t>Cndelta_a</t>
-  </si>
-  <si>
-    <t>Cndelta_r</t>
-  </si>
-  <si>
-    <t>CDiH</t>
-  </si>
-  <si>
-    <t>CLiH</t>
-  </si>
-  <si>
-    <t>CMiH</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Allowable System of Units</t>
-  </si>
-  <si>
-    <t>Imperial</t>
-  </si>
-  <si>
-    <t>Advanced Flight Dynamics - Nonlinear Flight Simulation</t>
-  </si>
-  <si>
-    <t>Current Version</t>
-  </si>
-  <si>
-    <t>1.0.0.11</t>
-  </si>
-  <si>
-    <t>System of Units</t>
-  </si>
-  <si>
-    <t>Advanced Flight Dynamics Nonlinear Flight Simulation is a comprehencive flight simulation (the Software simulation must goes here) …</t>
-  </si>
-  <si>
-    <t>MOI Tensor Rate</t>
+    <t>1.0.0.15</t>
   </si>
 </sst>
 </file>
@@ -367,7 +368,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,8 +425,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -491,6 +498,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -499,7 +552,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -545,9 +598,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -573,8 +623,26 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -588,17 +656,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -608,19 +685,12 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -634,6 +704,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -704,6 +788,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF2F2F2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -715,47 +804,23 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="AFD NFS"/>
-      <sheetName val="NFS Cruise - General Data"/>
-      <sheetName val="NFS Cruise - Aerodynamics Data"/>
-      <sheetName val="Prefered Data Sets"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="10">
-          <cell r="C10" t="str">
-            <v>Imperial</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:C14" headerRowCount="0" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:C14" headerRowCount="0" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <tableColumns count="3">
-    <tableColumn id="2" name="Column2" headerRowDxfId="9" dataDxfId="8"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="7" dataDxfId="6"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="5" dataDxfId="0"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="7" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:B27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <tableColumns count="2">
-    <tableColumn id="1" name="CD1" dataDxfId="2"/>
-    <tableColumn id="2" name="Column1" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:C27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <tableColumns count="3">
+    <tableColumn id="1" name="CD1" dataDxfId="3"/>
+    <tableColumn id="2" name="Column1" dataDxfId="2"/>
+    <tableColumn id="3" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1032,138 +1097,139 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="20"/>
-    <col min="2" max="2" width="16.3984375" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="8.8984375" style="20"/>
-    <col min="27" max="27" width="22.3984375" style="20" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.8984375" style="20"/>
+    <col min="1" max="1" width="8.8984375" style="19"/>
+    <col min="2" max="2" width="16.3984375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="8.8984375" style="19"/>
+    <col min="27" max="27" width="22.3984375" style="19" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.8984375" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="B5" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="B9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.65">
+      <c r="B10" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="B5" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="B9" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="B10" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
+      <c r="C10" s="30" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="AOi0XbhftgL7XjfxH1hv98vLjIion5kOqCOJhdHGbNh644cRVL/s+Ayt+1c2ir6UKmhNHp0HHUJqP0GPlZovcQ==" saltValue="507vXO68fRrbk8nSj1whcw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:L4"/>
     <mergeCell ref="B5:K8"/>
@@ -1183,7 +1249,7 @@
   <dimension ref="A1:Y203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1200,11 +1266,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="A1" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
@@ -1230,14 +1296,15 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="6">
-        <v>6360</v>
-      </c>
-      <c r="C2" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","lb","kg")</f>
-        <v>lb</v>
+        <v>86</v>
+      </c>
+      <c r="B2" s="31">
+        <f>1790.5*9.806</f>
+        <v>17557.643</v>
+      </c>
+      <c r="C2" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","lb","N")</f>
+        <v>N</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -1267,11 +1334,11 @@
         <v>10</v>
       </c>
       <c r="B3" s="6">
-        <v>30000</v>
-      </c>
-      <c r="C3" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","ft","m")</f>
-        <v>ft</v>
+        <v>10000</v>
+      </c>
+      <c r="C3" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","ft","m")</f>
+        <v>m</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -1301,11 +1368,11 @@
         <v>0</v>
       </c>
       <c r="B4" s="6">
-        <v>5.47</v>
-      </c>
-      <c r="C4" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","ft","m")</f>
-        <v>ft</v>
+        <v>1.0013170130787601</v>
+      </c>
+      <c r="C4" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","ft","m")</f>
+        <v>m</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -1335,11 +1402,11 @@
         <v>1</v>
       </c>
       <c r="B5" s="6">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="C5" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","ft","m")</f>
-        <v>ft</v>
+        <v>23.550000000772599</v>
+      </c>
+      <c r="C5" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","ft","m")</f>
+        <v>m</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -1369,11 +1436,11 @@
         <v>2</v>
       </c>
       <c r="B6" s="6">
-        <v>182</v>
-      </c>
-      <c r="C6" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","ft^2","m^2")</f>
-        <v>ft^2</v>
+        <v>11.790507829389201</v>
+      </c>
+      <c r="C6" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","ft^2","m^2")</f>
+        <v>m^2</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -1400,14 +1467,14 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="6">
-        <v>456</v>
-      </c>
-      <c r="C7" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","ft/sec","m/s")</f>
-        <v>ft/sec</v>
+        <v>69.897199999999998</v>
+      </c>
+      <c r="C7" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","ft/sec","m/s")</f>
+        <v>m/s</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -1437,11 +1504,11 @@
         <v>3</v>
       </c>
       <c r="B8" s="6">
-        <v>92.7</v>
-      </c>
-      <c r="C8" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","lb/ft^2","Pa")</f>
-        <v>lb/ft^2</v>
+        <v>1586.75</v>
+      </c>
+      <c r="C8" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","lb/ft^2","Pa")</f>
+        <v>Pa</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1473,8 +1540,8 @@
       <c r="B9" s="6">
         <v>0</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>16</v>
+      <c r="C9" s="23" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1506,9 +1573,9 @@
       <c r="B10" s="6">
         <v>0</v>
       </c>
-      <c r="C10" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","ft","m")</f>
-        <v>ft</v>
+      <c r="C10" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","ft","m")</f>
+        <v>m</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -1540,8 +1607,8 @@
       <c r="B11" s="6">
         <v>0</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>16</v>
+      <c r="C11" s="23" t="s">
+        <v>15</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -1573,8 +1640,8 @@
       <c r="B12" s="6">
         <v>0</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>16</v>
+      <c r="C12" s="23" t="s">
+        <v>15</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -1606,9 +1673,9 @@
       <c r="B13" s="6">
         <v>0</v>
       </c>
-      <c r="C13" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","lbs/sec","kg/s")</f>
-        <v>lbs/sec</v>
+      <c r="C13" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","lbs/sec","kg/s")</f>
+        <v>kg/s</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -1638,11 +1705,11 @@
         <v>9</v>
       </c>
       <c r="B14" s="6">
-        <v>32.174050000000001</v>
-      </c>
-      <c r="C14" s="26" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","ft/sec^2","m/s^2")</f>
-        <v>ft/sec^2</v>
+        <v>9.8010000000000002</v>
+      </c>
+      <c r="C14" s="23" t="str">
+        <f>IF('AFD NFS'!C10="Imperial","ft/sec^2","m/s^2")</f>
+        <v>m/s^2</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -1667,21 +1734,17 @@
       <c r="X14" s="14"/>
       <c r="Y14" s="14"/>
     </row>
-    <row r="15" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
+    <row r="15" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="18">
-        <v>7985</v>
-      </c>
-      <c r="C16" s="19">
-        <v>0</v>
-      </c>
-      <c r="D16" s="18">
-        <v>0</v>
+      <c r="B16" s="17">
+        <v>16095.043</v>
+      </c>
+      <c r="C16" s="18">
+        <v>21.74</v>
+      </c>
+      <c r="D16" s="17">
+        <v>-731.03399999999999</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1705,21 +1768,21 @@
       <c r="Y16" s="14"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="19">
-        <v>0</v>
-      </c>
-      <c r="C17" s="18">
-        <v>3326</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0</v>
+      <c r="A17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="18">
+        <v>21.74</v>
+      </c>
+      <c r="C17" s="17">
+        <v>8693.6</v>
+      </c>
+      <c r="D17" s="18">
+        <v>5.8639999999999999</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","slug*ft^2","kg.m^2")</f>
-        <v>slug*ft^2</v>
+        <f>IF('AFD NFS'!C10="Imperial","slug*ft^2","kg.m^2")</f>
+        <v>kg.m^2</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1744,14 +1807,14 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="19">
-        <v>0</v>
-      </c>
-      <c r="D18" s="18">
-        <v>11183</v>
+      <c r="B18" s="17">
+        <v>-731.03399999999999</v>
+      </c>
+      <c r="C18" s="18">
+        <v>5.8639999999999999</v>
+      </c>
+      <c r="D18" s="17">
+        <v>24181.062999999998</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
@@ -1777,9 +1840,9 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -1803,150 +1866,150 @@
       <c r="Y19" s="14"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="18">
+      <c r="A20" s="23"/>
+      <c r="B20" s="17">
         <v>0</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="18">
         <v>0</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="17">
         <v>0</v>
       </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="25"/>
-      <c r="U20" s="25"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="25"/>
-      <c r="X20" s="25"/>
-      <c r="Y20" s="25"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="24"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="19">
+      <c r="A21" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="18">
         <v>0</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="17">
         <v>0</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="18">
         <v>0</v>
       </c>
       <c r="E21" s="4" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","slug*ft^2","kg.m^2")</f>
-        <v>slug*ft^2</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="25"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="25"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="25"/>
+        <f>IF('AFD NFS'!C10="Imperial","slug*ft^2","kg.m^2")</f>
+        <v>kg.m^2</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="18">
+      <c r="A22" s="24"/>
+      <c r="B22" s="17">
         <v>0</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="18">
         <v>0</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>0</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="25"/>
-      <c r="U22" s="25"/>
-      <c r="V22" s="25"/>
-      <c r="W22" s="25"/>
-      <c r="X22" s="25"/>
-      <c r="Y22" s="25"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="24"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="25"/>
-      <c r="U23" s="25"/>
-      <c r="V23" s="25"/>
-      <c r="W23" s="25"/>
-      <c r="X23" s="25"/>
-      <c r="Y23" s="25"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="24"/>
+      <c r="Y23" s="24"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="18">
+        <v>13</v>
+      </c>
+      <c r="B24" s="17">
         <v>0</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="18">
         <v>0</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="17">
         <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1971,9 +2034,9 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -1997,20 +2060,20 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="19">
+        <v>14</v>
+      </c>
+      <c r="B26" s="18">
         <v>0</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="17">
         <v>0</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="18">
         <v>0</v>
       </c>
       <c r="E26" s="5" t="str">
-        <f>IF('[1]AFD NFS'!C10="Imperial","rad/sec","rad/s")</f>
-        <v>rad/sec</v>
+        <f>IF('AFD NFS'!C10="Imperial","rad/sec","rad/s")</f>
+        <v>rad/s</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -2211,6 +2274,7 @@
     <row r="202" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="203" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="zA4c3cyz23ZH8u8hLTLsDAslrCI3dS+asU3H/j9yJGT+JqEQOe/+SAJk70dfQ6uzuVQtKtz3+oQCXJvjgdqTYQ==" saltValue="eVDLF3cteQk/il8bD2J9xQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
@@ -2227,41 +2291,72 @@
   <dimension ref="A1:Z190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="184.8984375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.09765625" style="1"/>
+    <col min="3" max="3" width="13.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="163.8984375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.09765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="26"/>
+    </row>
+    <row r="2" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+    </row>
+    <row r="3" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="C4" s="9"/>
+        <v>5.5419999999999997E-2</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>83</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -2288,12 +2383,14 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="C5" s="9"/>
+        <v>1.111E-2</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -2320,12 +2417,14 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="7">
         <v>0</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -2352,12 +2451,14 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="C7" s="9"/>
+        <v>-9.1673247220931692E-3</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -2384,12 +2485,14 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7">
         <v>0</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -2416,12 +2519,14 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7">
-        <v>2.98E-2</v>
-      </c>
-      <c r="C9" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -2448,12 +2553,14 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="C10" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -2480,12 +2587,14 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="7">
-        <v>0.378</v>
-      </c>
-      <c r="C11" s="9"/>
+        <v>0.84494999999999998</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -2512,12 +2621,14 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="C12" s="9"/>
+        <v>0.44488</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -2544,12 +2655,14 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="7">
         <v>0</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -2576,12 +2689,14 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="7">
-        <v>5.15</v>
-      </c>
-      <c r="C14" s="9"/>
+        <v>7.8048310852720704</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -2608,12 +2723,14 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="7">
-        <v>2</v>
-      </c>
-      <c r="C15" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -2640,12 +2757,14 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="7">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C16" s="9"/>
+        <v>14.99699</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -2672,12 +2791,14 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="7">
         <v>0</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -2704,12 +2825,14 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="7">
         <v>0</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -2736,12 +2859,14 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="7">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C19" s="9"/>
+        <v>4.0849999999999997E-2</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -2768,12 +2893,14 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="7">
         <v>0</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -2800,12 +2927,14 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="7">
-        <v>-0.7</v>
-      </c>
-      <c r="C21" s="9"/>
+        <v>-1.4329674456221899</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -2832,12 +2961,14 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="7">
-        <v>-6.95</v>
-      </c>
-      <c r="C22" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -2864,12 +2995,14 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" s="7">
-        <v>-14.9</v>
-      </c>
-      <c r="C23" s="9"/>
+        <v>-27.884799999999998</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
@@ -2896,12 +3029,14 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" s="7">
         <v>0</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
@@ -2928,12 +3063,14 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" s="7">
         <v>0</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -2960,12 +3097,14 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" s="7">
         <v>0</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -2992,12 +3131,14 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="7">
         <v>0</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -3022,19 +3163,21 @@
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
     </row>
-    <row r="28" spans="1:26" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>68</v>
+    <row r="28" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="40" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B29" s="11">
-        <v>-0.34599999999999997</v>
-      </c>
-      <c r="C29" s="9"/>
+        <v>-1.0198648753328701</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -3061,12 +3204,14 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" s="13">
         <v>0</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -3093,12 +3238,14 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B31" s="11">
-        <v>-8.2699999999999996E-2</v>
-      </c>
-      <c r="C31" s="9"/>
+        <v>-8.0180000000000001E-2</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -3125,12 +3272,14 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B32" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="C32" s="9"/>
+        <v>0.25298999999999999</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
@@ -3157,12 +3306,14 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B33" s="11">
-        <v>-9.4399999999999998E-2</v>
-      </c>
-      <c r="C33" s="9"/>
+        <v>-1.4400000000000001E-3</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
@@ -3189,12 +3340,14 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B34" s="13">
         <v>0</v>
       </c>
-      <c r="C34" s="9"/>
+      <c r="C34" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -3221,12 +3374,14 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B35" s="11">
-        <v>-0.442</v>
-      </c>
-      <c r="C35" s="9"/>
+        <v>-0.82752999999999999</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
@@ -3253,12 +3408,14 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B36" s="13">
-        <v>9.2600000000000002E-2</v>
-      </c>
-      <c r="C36" s="9"/>
+        <v>2.4910000000000002E-2</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
@@ -3285,12 +3442,14 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B37" s="11">
-        <v>0.1106</v>
-      </c>
-      <c r="C37" s="9"/>
+        <v>8.8808458245277597E-2</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
@@ -3317,12 +3476,14 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B38" s="13">
         <v>0</v>
       </c>
-      <c r="C38" s="9"/>
+      <c r="C38" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -3349,12 +3510,14 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39" s="11">
-        <v>-2.4299999999999999E-2</v>
-      </c>
-      <c r="C39" s="9"/>
+        <v>1.256E-2</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
@@ -3381,12 +3544,14 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B40" s="13">
-        <v>-0.13900000000000001</v>
-      </c>
-      <c r="C40" s="9"/>
+        <v>-3.2219999999999999E-2</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -3413,12 +3578,14 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B41" s="11">
         <v>0</v>
       </c>
-      <c r="C41" s="9"/>
+      <c r="C41" s="27" t="s">
+        <v>83</v>
+      </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -3443,25 +3610,27 @@
       <c r="Y41" s="9"/>
       <c r="Z41" s="9"/>
     </row>
-    <row r="42" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
-        <v>21</v>
+    <row r="42" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="40" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B45" s="11">
-        <v>0</v>
-      </c>
-      <c r="C45" s="9"/>
+        <v>-5.1566201561774102E-3</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
@@ -3488,12 +3657,14 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B46" s="13">
         <v>0</v>
       </c>
-      <c r="C46" s="9"/>
+      <c r="C46" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
@@ -3520,12 +3691,14 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B47" s="11">
         <v>0</v>
       </c>
-      <c r="C47" s="9"/>
+      <c r="C47" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
@@ -3552,12 +3725,14 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B48" s="13">
         <v>0</v>
       </c>
-      <c r="C48" s="9"/>
+      <c r="C48" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -3584,12 +3759,14 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B49" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="C49" s="9"/>
+        <v>1.2817065877076499</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
@@ -3616,12 +3793,14 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B50" s="13">
-        <v>0</v>
-      </c>
-      <c r="C50" s="9"/>
+        <v>2.01509256547511</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
@@ -3648,12 +3827,14 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B51" s="11">
-        <v>-1.1200000000000001</v>
-      </c>
-      <c r="C51" s="9"/>
+        <v>-3.37987803347673</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
@@ -3680,12 +3861,14 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B52" s="13">
-        <v>0</v>
-      </c>
-      <c r="C52" s="9"/>
+        <v>0.37757918699121301</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
@@ -3712,12 +3895,14 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B53" s="11">
         <v>0</v>
       </c>
-      <c r="C53" s="9"/>
+      <c r="C53" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
@@ -3744,12 +3929,14 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B54" s="13">
         <v>0</v>
       </c>
-      <c r="C54" s="9"/>
+      <c r="C54" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
@@ -3776,12 +3963,14 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B55" s="11">
         <v>0</v>
       </c>
-      <c r="C55" s="9"/>
+      <c r="C55" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
@@ -3806,19 +3995,21 @@
       <c r="Y55" s="9"/>
       <c r="Z55" s="9"/>
     </row>
-    <row r="56" spans="1:26" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="32" t="s">
-        <v>68</v>
+    <row r="56" spans="1:26" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="40" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B57" s="11">
-        <v>0</v>
-      </c>
-      <c r="C57" s="14"/>
+        <v>5.7295779513082297E-3</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
@@ -3845,12 +4036,14 @@
     </row>
     <row r="58" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B58" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="C58" s="14"/>
+        <v>0.16673071838306999</v>
+      </c>
+      <c r="C58" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
@@ -3877,12 +4070,14 @@
     </row>
     <row r="59" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B59" s="11">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="C59" s="14"/>
+        <v>0.39935158320618402</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -3909,12 +4104,14 @@
     </row>
     <row r="60" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B60" s="13">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="C60" s="14"/>
+        <v>5.7295779513082297E-4</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -3941,12 +4138,14 @@
     </row>
     <row r="61" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B61" s="11">
-        <v>-2.5399999999999999E-2</v>
-      </c>
-      <c r="C61" s="14"/>
+        <v>-5.7295779513082297E-4</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
@@ -3973,12 +4172,14 @@
     </row>
     <row r="62" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B62" s="13">
-        <v>-3.6499999999999998E-2</v>
-      </c>
-      <c r="C62" s="14"/>
+        <v>-2.0626480624709599E-2</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>84</v>
+      </c>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
@@ -4003,8 +4204,8 @@
       <c r="Y62" s="14"/>
       <c r="Z62" s="14"/>
     </row>
-    <row r="63" spans="1:26" s="31" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:26" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:26" s="39" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
@@ -4144,17 +4345,18 @@
       <c r="B190" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mEd+ZgXKJg+QgyEqtreW8e02kRKtIxmAASAWRJeXuwH8Ap9Ttb1ddy3cLq+sHmjK6Z7ay9ukyEGswnLHDDd9QQ==" saltValue="2gJuk89JV9p1RQEADiqAZQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="9">
+  <sheetProtection algorithmName="SHA-512" hashValue="a9uhngi7BUM6YTnwhPHRq5raDq9s9secGpDYdppcGvqmt7j3yLrDQV6qHzpKLKyZSprp6Lal5Y63yC1nXu61HQ==" saltValue="cjH/Rx7HngGDE6guwpng0w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="A64:XFD64"/>
     <mergeCell ref="A63:XFD63"/>
     <mergeCell ref="A44:XFD44"/>
     <mergeCell ref="A56:XFD56"/>
-    <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A3:XFD3"/>
     <mergeCell ref="A28:XFD28"/>
     <mergeCell ref="A43:XFD43"/>
+    <mergeCell ref="A42:XFD42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4178,17 +4380,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.65">
-      <c r="A1" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.65">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.65">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Some Filters something is WRONG with g Check that out
turbulence models became variant subsystem
some other minor changes
</commit_message>
<xml_diff>
--- a/NFSData/NFS Data.xlsx
+++ b/NFSData/NFS Data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="M0R0OALV+6f4UVn5GwSJvjPKd6y0Z7YAv336xc5+wD0694sFyycXUoMm4kQWjCbyA7IyUV/m+S/8rCX45lhMVg==" workbookSaltValue="i7Ezyq5BRvQUEGVk7PYG3A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23976" windowHeight="10260" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23976" windowHeight="10260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AFD NFS" sheetId="4" r:id="rId1"/>
@@ -685,29 +685,14 @@
   <dxfs count="14">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -734,6 +719,21 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -805,19 +805,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:C14" headerRowCount="0" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <tableColumns count="3">
     <tableColumn id="2" name="Column2" headerRowDxfId="11" dataDxfId="10"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="9" dataDxfId="1"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="8" dataDxfId="7"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="7" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:C27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:C27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="3">
-    <tableColumn id="1" name="CD1" dataDxfId="4"/>
-    <tableColumn id="2" name="Column1" dataDxfId="0"/>
-    <tableColumn id="3" name="Column2" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="1" name="CD1" dataDxfId="3"/>
+    <tableColumn id="2" name="Column1" dataDxfId="2"/>
+    <tableColumn id="3" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,7 @@
         <v>86</v>
       </c>
       <c r="B2" s="6">
-        <v>6360</v>
+        <v>6336.0872381425897</v>
       </c>
       <c r="C2" s="23" t="str">
         <f>IF('AFD NFS'!C10="Imperial","lb","N")</f>
@@ -1701,7 +1701,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="6">
-        <v>32.174050000000001</v>
+        <v>32.053030612967802</v>
       </c>
       <c r="C14" s="23" t="str">
         <f>IF('AFD NFS'!C10="Imperial","ft/sec^2","m/s^2")</f>
@@ -2286,7 +2286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B57" sqref="B57:B62"/>
     </sheetView>

</xml_diff>

<commit_message>
Some Major Changes to include lateral directional dynamics in trim
</commit_message>
<xml_diff>
--- a/NFSData/NFS Data.xlsx
+++ b/NFSData/NFS Data.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\A.H.Kh\HomeWork\04-Practical Projects\AFDNFS\AFDNFS Git\NFSData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE6306D-3B71-4997-B304-3FD0172D676A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="M0R0OALV+6f4UVn5GwSJvjPKd6y0Z7YAv336xc5+wD0694sFyycXUoMm4kQWjCbyA7IyUV/m+S/8rCX45lhMVg==" workbookSaltValue="i7Ezyq5BRvQUEGVk7PYG3A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23976" windowHeight="10260" activeTab="1"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AFD NFS" sheetId="4" r:id="rId1"/>
@@ -21,10 +22,16 @@
   <definedNames>
     <definedName name="Units">'Prefered Data Sets'!$B$1:$B$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -300,33 +307,33 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="4" tint="-0.499984740745262"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -334,14 +341,14 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.499984740745262"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,7 +356,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -802,22 +809,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:C14" headerRowCount="0" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A2:C14" headerRowCount="0" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <tableColumns count="3">
-    <tableColumn id="2" name="Column2" headerRowDxfId="11" dataDxfId="10"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="9" dataDxfId="8"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" headerRowDxfId="7" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:C27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A5:C27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="3">
-    <tableColumn id="1" name="CD1" dataDxfId="3"/>
-    <tableColumn id="2" name="Column1" dataDxfId="2"/>
-    <tableColumn id="3" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CD1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1085,20 +1092,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="19"/>
-    <col min="2" max="2" width="16.3984375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="8.8984375" style="19"/>
-    <col min="27" max="27" width="22.3984375" style="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.8984375" style="19"/>
+    <col min="1" max="1" width="8.88671875" style="19"/>
+    <col min="2" max="2" width="16.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="8.88671875" style="19"/>
+    <col min="27" max="27" width="22.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.65">
@@ -1232,7 +1239,7 @@
     <mergeCell ref="B5:K8"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Units</formula1>
     </dataValidation>
   </dataValidations>
@@ -1242,27 +1249,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.09765625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.09765625" style="2"/>
-    <col min="6" max="6" width="152.296875" style="2" customWidth="1"/>
-    <col min="7" max="8" width="9.09765625" style="2"/>
-    <col min="9" max="10" width="28.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2"/>
+    <col min="6" max="6" width="152.33203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" style="2"/>
+    <col min="9" max="10" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.09765625" style="2"/>
+    <col min="13" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
@@ -1291,7 +1298,7 @@
       <c r="X1" s="14"/>
       <c r="Y1" s="14"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
@@ -1325,7 +1332,7 @@
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1359,7 +1366,7 @@
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1400,7 @@
       <c r="X4" s="14"/>
       <c r="Y4" s="14"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1427,7 +1434,7 @@
       <c r="X5" s="14"/>
       <c r="Y5" s="14"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1461,7 +1468,7 @@
       <c r="X6" s="14"/>
       <c r="Y6" s="14"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1495,7 +1502,7 @@
       <c r="X7" s="14"/>
       <c r="Y7" s="14"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1529,12 +1536,12 @@
       <c r="X8" s="14"/>
       <c r="Y8" s="14"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="6">
-        <v>0</v>
+        <v>-0.32174999999999998</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>15</v>
@@ -1562,7 +1569,7 @@
       <c r="X9" s="14"/>
       <c r="Y9" s="14"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1596,7 +1603,7 @@
       <c r="X10" s="14"/>
       <c r="Y10" s="14"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1629,7 +1636,7 @@
       <c r="X11" s="14"/>
       <c r="Y11" s="14"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1662,7 +1669,7 @@
       <c r="X12" s="14"/>
       <c r="Y12" s="14"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1696,7 +1703,7 @@
       <c r="X13" s="14"/>
       <c r="Y13" s="14"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1730,8 +1737,8 @@
       <c r="X14" s="14"/>
       <c r="Y14" s="14"/>
     </row>
-    <row r="15" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="17">
         <v>7985</v>
@@ -1763,7 +1770,7 @@
       <c r="X16" s="14"/>
       <c r="Y16" s="14"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>12</v>
       </c>
@@ -1801,7 +1808,7 @@
       <c r="X17" s="14"/>
       <c r="Y17" s="14"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="17">
         <v>0</v>
@@ -1834,7 +1841,7 @@
       <c r="X18" s="14"/>
       <c r="Y18" s="14"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -1861,7 +1868,7 @@
       <c r="X19" s="14"/>
       <c r="Y19" s="14"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="17">
         <v>0</v>
@@ -1893,7 +1900,7 @@
       <c r="X20" s="24"/>
       <c r="Y20" s="24"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>85</v>
       </c>
@@ -1931,7 +1938,7 @@
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="24"/>
       <c r="B22" s="17">
         <v>0</v>
@@ -1964,7 +1971,7 @@
       <c r="X22" s="24"/>
       <c r="Y22" s="24"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="24"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1991,7 +1998,7 @@
       <c r="X23" s="24"/>
       <c r="Y23" s="24"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
@@ -2028,7 +2035,7 @@
       <c r="X24" s="14"/>
       <c r="Y24" s="14"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2054,7 +2061,7 @@
       <c r="X25" s="14"/>
       <c r="Y25" s="14"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -2092,183 +2099,183 @@
       <c r="X26" s="14"/>
       <c r="Y26" s="14"/>
     </row>
-    <row r="27" spans="1:25" s="14" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="155" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="156" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="157" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="158" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="159" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="162" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="164" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="165" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="166" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="167" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="168" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="169" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="170" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="171" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="172" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="173" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="174" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="175" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="176" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="177" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="178" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="179" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="180" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="181" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="182" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="183" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="184" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="185" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="186" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="187" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="188" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="189" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="190" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="191" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="192" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="193" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="194" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="195" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="196" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="197" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="198" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="199" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="200" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="201" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="202" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="203" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:25" s="14" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="148" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="149" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="150" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="151" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="152" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="153" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="154" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="155" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="156" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="157" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="158" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="159" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="160" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="161" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="162" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="163" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="164" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="165" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="166" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="167" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="168" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="169" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="170" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="171" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="172" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="173" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="174" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="175" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="176" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="177" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="178" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="179" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="180" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="181" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="182" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="183" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="184" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="185" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="186" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="187" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="188" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="189" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="190" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="191" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="192" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="193" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="194" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="195" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="196" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="197" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="198" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="199" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="200" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="201" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="202" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="203" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="zA4c3cyz23ZH8u8hLTLsDAslrCI3dS+asU3H/j9yJGT+JqEQOe/+SAJk70dfQ6uzuVQtKtz3+oQCXJvjgdqTYQ==" saltValue="eVDLF3cteQk/il8bD2J9xQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
@@ -2283,7 +2290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2291,16 +2298,16 @@
       <selection pane="bottomLeft" activeCell="B57" sqref="B57:B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="163.8984375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.09765625" style="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="163.88671875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>17</v>
       </c>
@@ -2308,7 +2315,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>18</v>
       </c>
@@ -2338,12 +2345,12 @@
       <c r="Y2" s="40"/>
       <c r="Z2" s="40"/>
     </row>
-    <row r="3" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
@@ -2377,7 +2384,7 @@
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -2411,7 +2418,7 @@
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2445,7 +2452,7 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2479,7 +2486,7 @@
       <c r="Y7" s="9"/>
       <c r="Z7" s="9"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -2513,7 +2520,7 @@
       <c r="Y8" s="9"/>
       <c r="Z8" s="9"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2547,7 +2554,7 @@
       <c r="Y9" s="9"/>
       <c r="Z9" s="9"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -2581,7 +2588,7 @@
       <c r="Y10" s="9"/>
       <c r="Z10" s="9"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -2615,7 +2622,7 @@
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -2649,7 +2656,7 @@
       <c r="Y12" s="9"/>
       <c r="Z12" s="9"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
@@ -2683,7 +2690,7 @@
       <c r="Y13" s="9"/>
       <c r="Z13" s="9"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -2717,7 +2724,7 @@
       <c r="Y14" s="9"/>
       <c r="Z14" s="9"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -2751,7 +2758,7 @@
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -2785,7 +2792,7 @@
       <c r="Y16" s="9"/>
       <c r="Z16" s="9"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -2819,7 +2826,7 @@
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -2853,7 +2860,7 @@
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -2887,7 +2894,7 @@
       <c r="Y19" s="9"/>
       <c r="Z19" s="9"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -2921,7 +2928,7 @@
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -2955,7 +2962,7 @@
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -2989,7 +2996,7 @@
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
@@ -3023,7 +3030,7 @@
       <c r="Y23" s="9"/>
       <c r="Z23" s="9"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -3057,7 +3064,7 @@
       <c r="Y24" s="9"/>
       <c r="Z24" s="9"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
@@ -3091,7 +3098,7 @@
       <c r="Y25" s="9"/>
       <c r="Z25" s="9"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
@@ -3125,7 +3132,7 @@
       <c r="Y26" s="9"/>
       <c r="Z26" s="9"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
@@ -3159,12 +3166,12 @@
       <c r="Y27" s="9"/>
       <c r="Z27" s="9"/>
     </row>
-    <row r="28" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="39" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>44</v>
       </c>
@@ -3198,7 +3205,7 @@
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>45</v>
       </c>
@@ -3232,7 +3239,7 @@
       <c r="Y30" s="9"/>
       <c r="Z30" s="9"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>46</v>
       </c>
@@ -3266,7 +3273,7 @@
       <c r="Y31" s="9"/>
       <c r="Z31" s="9"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>47</v>
       </c>
@@ -3300,7 +3307,7 @@
       <c r="Y32" s="9"/>
       <c r="Z32" s="9"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -3334,7 +3341,7 @@
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>49</v>
       </c>
@@ -3368,7 +3375,7 @@
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -3402,7 +3409,7 @@
       <c r="Y35" s="9"/>
       <c r="Z35" s="9"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>51</v>
       </c>
@@ -3436,7 +3443,7 @@
       <c r="Y36" s="9"/>
       <c r="Z36" s="9"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -3470,7 +3477,7 @@
       <c r="Y37" s="9"/>
       <c r="Z37" s="9"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>53</v>
       </c>
@@ -3504,7 +3511,7 @@
       <c r="Y38" s="9"/>
       <c r="Z38" s="9"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>54</v>
       </c>
@@ -3538,7 +3545,7 @@
       <c r="Y39" s="9"/>
       <c r="Z39" s="9"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>55</v>
       </c>
@@ -3572,7 +3579,7 @@
       <c r="Y40" s="9"/>
       <c r="Z40" s="9"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>56</v>
       </c>
@@ -3606,18 +3613,18 @@
       <c r="Y41" s="9"/>
       <c r="Z41" s="9"/>
     </row>
-    <row r="42" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="39" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>58</v>
       </c>
@@ -3651,7 +3658,7 @@
       <c r="Y45" s="9"/>
       <c r="Z45" s="9"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>59</v>
       </c>
@@ -3685,7 +3692,7 @@
       <c r="Y46" s="9"/>
       <c r="Z46" s="9"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>60</v>
       </c>
@@ -3719,7 +3726,7 @@
       <c r="Y47" s="9"/>
       <c r="Z47" s="9"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>61</v>
       </c>
@@ -3753,7 +3760,7 @@
       <c r="Y48" s="9"/>
       <c r="Z48" s="9"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>62</v>
       </c>
@@ -3787,7 +3794,7 @@
       <c r="Y49" s="9"/>
       <c r="Z49" s="9"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>63</v>
       </c>
@@ -3821,7 +3828,7 @@
       <c r="Y50" s="9"/>
       <c r="Z50" s="9"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>64</v>
       </c>
@@ -3855,7 +3862,7 @@
       <c r="Y51" s="9"/>
       <c r="Z51" s="9"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>65</v>
       </c>
@@ -3889,7 +3896,7 @@
       <c r="Y52" s="9"/>
       <c r="Z52" s="9"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>73</v>
       </c>
@@ -3923,7 +3930,7 @@
       <c r="Y53" s="9"/>
       <c r="Z53" s="9"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>74</v>
       </c>
@@ -3957,7 +3964,7 @@
       <c r="Y54" s="9"/>
       <c r="Z54" s="9"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>75</v>
       </c>
@@ -3991,12 +3998,12 @@
       <c r="Y55" s="9"/>
       <c r="Z55" s="9"/>
     </row>
-    <row r="56" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="39" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>67</v>
       </c>
@@ -4030,7 +4037,7 @@
       <c r="Y57" s="14"/>
       <c r="Z57" s="14"/>
     </row>
-    <row r="58" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
         <v>68</v>
       </c>
@@ -4064,7 +4071,7 @@
       <c r="Y58" s="14"/>
       <c r="Z58" s="14"/>
     </row>
-    <row r="59" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>69</v>
       </c>
@@ -4098,7 +4105,7 @@
       <c r="Y59" s="14"/>
       <c r="Z59" s="14"/>
     </row>
-    <row r="60" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
         <v>70</v>
       </c>
@@ -4132,7 +4139,7 @@
       <c r="Y60" s="14"/>
       <c r="Z60" s="14"/>
     </row>
-    <row r="61" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>71</v>
       </c>
@@ -4166,7 +4173,7 @@
       <c r="Y61" s="14"/>
       <c r="Z61" s="14"/>
     </row>
-    <row r="62" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
         <v>72</v>
       </c>
@@ -4200,143 +4207,143 @@
       <c r="Y62" s="14"/>
       <c r="Z62" s="14"/>
     </row>
-    <row r="63" spans="1:26" s="38" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" s="38" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:26" s="38" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
     </row>
-    <row r="66" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
     </row>
-    <row r="67" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="155" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="156" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="157" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="158" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="159" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="162" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="164" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="165" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="166" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="167" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="168" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="169" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="170" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="171" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="172" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="173" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="174" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="175" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="176" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="180" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="182" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="183" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="184" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="185" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="186" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="187" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="188" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="189" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="148" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="149" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="150" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="151" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="152" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="153" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="154" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="155" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="156" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="157" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="158" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="159" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="160" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="161" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="162" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="163" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="164" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="165" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="166" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="167" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="168" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="169" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="170" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="171" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="172" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="173" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="174" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="175" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="176" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="177" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="178" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="179" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="180" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="181" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="182" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="183" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="184" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="185" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="186" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="187" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="188" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="189" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
     </row>
-    <row r="190" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
     </row>
@@ -4363,16 +4370,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.65">

</xml_diff>